<commit_message>
Updated w/ sig mucin
</commit_message>
<xml_diff>
--- a/mucin/mucinEnzymes.xlsx
+++ b/mucin/mucinEnzymes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/OG_MetaG/mucin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:40009_{7448471E-D2E7-45DB-8DF6-CCE832D2BC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E0C6467A-142C-4296-8A6C-EB6099CD5B06}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:40009_{7448471E-D2E7-45DB-8DF6-CCE832D2BC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE08306E-A4CA-4BC3-884C-65DF207C89BB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1229,12 +1229,13 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="17" max="17" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1389,7 +1390,7 @@
       <c r="P4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="7" t="s">
         <v>108</v>
       </c>
       <c r="R4">
@@ -1668,7 +1669,7 @@
       <c r="P11" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="7" t="s">
         <v>106</v>
       </c>
       <c r="R11">
@@ -1865,7 +1866,7 @@
       <c r="P16" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="7" t="s">
         <v>107</v>
       </c>
       <c r="R16">
@@ -2051,7 +2052,7 @@
       <c r="P21" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="7" t="s">
         <v>107</v>
       </c>
       <c r="R21">

</xml_diff>

<commit_message>
Something, not sure what
</commit_message>
<xml_diff>
--- a/mucin/mucinEnzymes.xlsx
+++ b/mucin/mucinEnzymes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/OG_MetaG/mucin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:40009_{7448471E-D2E7-45DB-8DF6-CCE832D2BC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE08306E-A4CA-4BC3-884C-65DF207C89BB}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:40009_{7448471E-D2E7-45DB-8DF6-CCE832D2BC84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F3458B63-093D-4B75-A224-CFD297121E9A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mucinEnzymes" sheetId="1" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>Bacteroidaceae, Muribaculaceae, Tannerellaceae</t>
   </si>
   <si>
-    <t>Bacteroidaceae, P{revotellaceae, Tannerellaceae</t>
-  </si>
-  <si>
     <t>Bacteroidaceae, Muribaculaceae, Clostridiaceae</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>AOV Pval</t>
+  </si>
+  <si>
+    <t>Bacteroidaceae, Prevotellaceae, Tannerellaceae</t>
   </si>
 </sst>
 </file>
@@ -1229,16 +1229,17 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="17" max="17" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="13" max="13" width="50.5703125" customWidth="1"/>
+    <col min="17" max="17" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,16 +1268,16 @@
         <v>88</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>87</v>
       </c>
       <c r="M2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R2">
         <v>0.224</v>
@@ -1317,7 +1318,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>83</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R4">
         <v>8.2000000000000007E-3</v>
@@ -1400,7 +1401,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1520,7 +1521,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>74</v>
       </c>
       <c r="M8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R8">
         <v>1.4500000000000001E-2</v>
@@ -1558,7 +1559,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>75</v>
       </c>
       <c r="M9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R9">
         <v>4.1099999999999998E-2</v>
@@ -1596,7 +1597,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1664,13 +1665,13 @@
         <v>70</v>
       </c>
       <c r="M11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P11" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R11">
         <v>7.7400000000000004E-3</v>
@@ -1682,7 +1683,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R12">
         <v>3.0200000000000001E-2</v>
@@ -1723,7 +1724,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>79</v>
       </c>
       <c r="M14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R14">
         <v>0.13300000000000001</v>
@@ -1797,7 +1798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1826,13 +1827,13 @@
         <v>74</v>
       </c>
       <c r="M15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R15">
         <v>7.5300000000000006E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1861,19 +1862,19 @@
         <v>70</v>
       </c>
       <c r="M16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P16" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R16">
         <v>8.1899999999999994E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1945,7 +1946,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2012,13 +2013,13 @@
         <v>81</v>
       </c>
       <c r="M20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R20">
         <v>2.2700000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2047,20 +2048,20 @@
         <v>82</v>
       </c>
       <c r="M21" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="P21" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R21">
         <v>1.9499999999999999E-3</v>
       </c>
       <c r="S21" s="5"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>7.8899999999999998E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
     </row>
   </sheetData>

</xml_diff>